<commit_message>
feat: readme with indication about challenge, solution, installations and executions
</commit_message>
<xml_diff>
--- a/tests/files/correct_data.xlsx
+++ b/tests/files/correct_data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="42">
   <si>
     <t>Surcharge</t>
   </si>
@@ -37,31 +37,34 @@
     <t>BL Fee</t>
   </si>
   <si>
+    <t>MSC--</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>freight</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>CMA CGM</t>
+  </si>
+  <si>
+    <t>MAERSK</t>
+  </si>
+  <si>
+    <t>Bill of Lading (BL)</t>
+  </si>
+  <si>
+    <t>YML</t>
+  </si>
+  <si>
+    <t>Ocean Freight</t>
+  </si>
+  <si>
     <t>MSC</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>freight</t>
-  </si>
-  <si>
-    <t>BL</t>
-  </si>
-  <si>
-    <t>CMA CGM</t>
-  </si>
-  <si>
-    <t>MAERSK</t>
-  </si>
-  <si>
-    <t>Bill of Lading (BL)</t>
-  </si>
-  <si>
-    <t>YML</t>
-  </si>
-  <si>
-    <t>Ocean Freight</t>
   </si>
   <si>
     <t>Ocean Freight Charge</t>
@@ -147,10 +150,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -189,6 +192,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
@@ -211,8 +222,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -227,15 +274,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -249,88 +334,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -347,19 +350,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -371,151 +506,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,6 +535,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -550,15 +564,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -570,6 +575,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -592,19 +606,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -623,157 +635,148 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1047,7 +1050,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6333333333333" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
@@ -1146,7 +1149,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3">
         <v>1000</v>
@@ -1160,7 +1163,7 @@
     </row>
     <row r="7" ht="12.75" customHeight="1" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
@@ -1194,7 +1197,7 @@
     </row>
     <row r="9" ht="12.75" customHeight="1" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>13</v>
@@ -1211,10 +1214,10 @@
     </row>
     <row r="10" ht="12.75" customHeight="1" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C10" s="3">
         <v>100</v>
@@ -1223,12 +1226,12 @@
         <v>7</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>10</v>
@@ -1240,12 +1243,12 @@
         <v>7</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>11</v>
@@ -1257,12 +1260,12 @@
         <v>7</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>13</v>
@@ -1274,15 +1277,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C14" s="3">
         <v>120</v>
@@ -1291,12 +1294,12 @@
         <v>7</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>10</v>
@@ -1308,12 +1311,12 @@
         <v>7</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>11</v>
@@ -1325,12 +1328,12 @@
         <v>7</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>13</v>
@@ -1342,15 +1345,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C18" s="3">
         <v>50</v>
@@ -1364,7 +1367,7 @@
     </row>
     <row r="19" ht="12.75" customHeight="1" spans="1:5">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>10</v>
@@ -1381,7 +1384,7 @@
     </row>
     <row r="20" ht="12.75" customHeight="1" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>11</v>
@@ -1398,7 +1401,7 @@
     </row>
     <row r="21" ht="12.75" customHeight="1" spans="1:5">
       <c r="A21" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>13</v>
@@ -1415,10 +1418,10 @@
     </row>
     <row r="22" ht="12.75" customHeight="1" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C22" s="3">
         <v>50</v>
@@ -1427,12 +1430,12 @@
         <v>7</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>10</v>
@@ -1444,12 +1447,12 @@
         <v>7</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>11</v>
@@ -1461,12 +1464,12 @@
         <v>7</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>13</v>
@@ -1478,15 +1481,15 @@
         <v>7</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1" spans="1:5">
       <c r="A26" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C26" s="3">
         <v>20</v>
@@ -1495,12 +1498,12 @@
         <v>7</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>10</v>
@@ -1517,7 +1520,7 @@
     </row>
     <row r="28" ht="12.75" customHeight="1" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>11</v>
@@ -1534,7 +1537,7 @@
     </row>
     <row r="29" ht="12.75" customHeight="1" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>13</v>
@@ -1551,10 +1554,10 @@
     </row>
     <row r="30" ht="12.75" customHeight="1" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C30" s="3">
         <v>50</v>
@@ -1568,7 +1571,7 @@
     </row>
     <row r="31" ht="12.75" customHeight="1" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>11</v>
@@ -1585,7 +1588,7 @@
     </row>
     <row r="32" ht="12.75" customHeight="1" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>13</v>
@@ -1602,10 +1605,10 @@
     </row>
     <row r="33" ht="12.75" customHeight="1" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C33" s="3">
         <v>30</v>
@@ -1619,10 +1622,10 @@
     </row>
     <row r="34" ht="12.75" customHeight="1" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C34" s="3">
         <v>100</v>
@@ -1631,15 +1634,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" ht="12.75" customHeight="1" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C35" s="3">
         <v>105</v>
@@ -1648,12 +1651,12 @@
         <v>7</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" ht="12.75" customHeight="1" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>11</v>
@@ -1665,15 +1668,15 @@
         <v>7</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" ht="12.75" customHeight="1" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C37" s="3">
         <v>120</v>
@@ -1682,15 +1685,15 @@
         <v>7</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C38" s="3">
         <v>200</v>
@@ -1704,10 +1707,10 @@
     </row>
     <row r="39" ht="12.75" customHeight="1" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C39" s="3">
         <v>200</v>
@@ -1721,7 +1724,7 @@
     </row>
     <row r="40" ht="12.75" customHeight="1" spans="1:5">
       <c r="A40" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>10</v>
@@ -1738,10 +1741,10 @@
     </row>
     <row r="41" ht="12.75" customHeight="1" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C41" s="3">
         <v>80</v>
@@ -1750,12 +1753,12 @@
         <v>7</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" ht="12.75" customHeight="1" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>10</v>
@@ -1767,15 +1770,15 @@
         <v>7</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" ht="12.75" customHeight="1" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C43" s="3">
         <v>95</v>
@@ -1784,7 +1787,7 @@
         <v>7</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" ht="12.75" customHeight="1"/>

</xml_diff>

<commit_message>
chore: other tests about rates
</commit_message>
<xml_diff>
--- a/tests/files/correct_data.xlsx
+++ b/tests/files/correct_data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="41">
   <si>
     <t>Surcharge</t>
   </si>
@@ -37,7 +37,7 @@
     <t>BL Fee</t>
   </si>
   <si>
-    <t>MSC--</t>
+    <t>MSC</t>
   </si>
   <si>
     <t>USD</t>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>Ocean Freight</t>
-  </si>
-  <si>
-    <t>MSC</t>
   </si>
   <si>
     <t>Ocean Freight Charge</t>
@@ -150,10 +147,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -184,17 +181,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,27 +213,19 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
@@ -244,25 +240,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -274,25 +256,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -305,15 +271,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,13 +310,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -344,187 +341,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -535,17 +532,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -560,6 +546,24 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -605,18 +609,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -638,148 +635,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1149,7 +1146,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3">
         <v>1000</v>
@@ -1163,7 +1160,7 @@
     </row>
     <row r="7" ht="12.75" customHeight="1" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
@@ -1197,7 +1194,7 @@
     </row>
     <row r="9" ht="12.75" customHeight="1" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>13</v>
@@ -1214,10 +1211,10 @@
     </row>
     <row r="10" ht="12.75" customHeight="1" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C10" s="3">
         <v>100</v>
@@ -1226,12 +1223,12 @@
         <v>7</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>10</v>
@@ -1243,12 +1240,12 @@
         <v>7</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>11</v>
@@ -1260,12 +1257,12 @@
         <v>7</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>13</v>
@@ -1277,15 +1274,15 @@
         <v>7</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C14" s="3">
         <v>120</v>
@@ -1294,12 +1291,12 @@
         <v>7</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>10</v>
@@ -1311,12 +1308,12 @@
         <v>7</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>11</v>
@@ -1328,12 +1325,12 @@
         <v>7</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>13</v>
@@ -1345,15 +1342,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C18" s="3">
         <v>50</v>
@@ -1367,7 +1364,7 @@
     </row>
     <row r="19" ht="12.75" customHeight="1" spans="1:5">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>10</v>
@@ -1384,7 +1381,7 @@
     </row>
     <row r="20" ht="12.75" customHeight="1" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>11</v>
@@ -1401,7 +1398,7 @@
     </row>
     <row r="21" ht="12.75" customHeight="1" spans="1:5">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>13</v>
@@ -1418,10 +1415,10 @@
     </row>
     <row r="22" ht="12.75" customHeight="1" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C22" s="3">
         <v>50</v>
@@ -1430,12 +1427,12 @@
         <v>7</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>10</v>
@@ -1447,12 +1444,12 @@
         <v>7</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>11</v>
@@ -1464,12 +1461,12 @@
         <v>7</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>13</v>
@@ -1481,15 +1478,15 @@
         <v>7</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1" spans="1:5">
       <c r="A26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="C26" s="3">
         <v>20</v>
@@ -1498,12 +1495,12 @@
         <v>7</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>10</v>
@@ -1520,7 +1517,7 @@
     </row>
     <row r="28" ht="12.75" customHeight="1" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>11</v>
@@ -1537,7 +1534,7 @@
     </row>
     <row r="29" ht="12.75" customHeight="1" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>13</v>
@@ -1554,10 +1551,10 @@
     </row>
     <row r="30" ht="12.75" customHeight="1" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" s="3">
         <v>50</v>
@@ -1571,7 +1568,7 @@
     </row>
     <row r="31" ht="12.75" customHeight="1" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>11</v>
@@ -1588,7 +1585,7 @@
     </row>
     <row r="32" ht="12.75" customHeight="1" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>13</v>
@@ -1605,10 +1602,10 @@
     </row>
     <row r="33" ht="12.75" customHeight="1" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C33" s="3">
         <v>30</v>
@@ -1622,10 +1619,10 @@
     </row>
     <row r="34" ht="12.75" customHeight="1" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C34" s="3">
         <v>100</v>
@@ -1634,15 +1631,15 @@
         <v>7</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" ht="12.75" customHeight="1" spans="1:5">
       <c r="A35" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="C35" s="3">
         <v>105</v>
@@ -1651,12 +1648,12 @@
         <v>7</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" ht="12.75" customHeight="1" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>11</v>
@@ -1668,15 +1665,15 @@
         <v>7</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" ht="12.75" customHeight="1" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C37" s="3">
         <v>120</v>
@@ -1685,15 +1682,15 @@
         <v>7</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1" spans="1:5">
       <c r="A38" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="C38" s="3">
         <v>200</v>
@@ -1707,10 +1704,10 @@
     </row>
     <row r="39" ht="12.75" customHeight="1" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39" s="3">
         <v>200</v>
@@ -1724,7 +1721,7 @@
     </row>
     <row r="40" ht="12.75" customHeight="1" spans="1:5">
       <c r="A40" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>10</v>
@@ -1741,10 +1738,10 @@
     </row>
     <row r="41" ht="12.75" customHeight="1" spans="1:5">
       <c r="A41" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" s="3">
         <v>80</v>
@@ -1753,12 +1750,12 @@
         <v>7</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" ht="12.75" customHeight="1" spans="1:5">
       <c r="A42" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>10</v>
@@ -1770,15 +1767,15 @@
         <v>7</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" ht="12.75" customHeight="1" spans="1:5">
       <c r="A43" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C43" s="3">
         <v>95</v>
@@ -1787,7 +1784,7 @@
         <v>7</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" ht="12.75" customHeight="1"/>

</xml_diff>